<commit_message>
Diapo de présentation à modifier si vou voulez rajouter des trucs
</commit_message>
<xml_diff>
--- a/Documents/Exigence-fonctionnel.xlsx
+++ b/Documents/Exigence-fonctionnel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC2B3DEA-58E0-4A71-BF5B-60DCE50CF74B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74108435-FBED-45D6-9A5E-63434BDC0850}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
   <si>
     <t>EF_001</t>
   </si>
@@ -605,6 +605,15 @@
   </si>
   <si>
     <t xml:space="preserve">Affichage d'un bouton rejoindre </t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Marion</t>
   </si>
 </sst>
 </file>
@@ -974,13 +983,13 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5546875" customWidth="1"/>
-    <col min="2" max="2" width="134" customWidth="1"/>
+    <col min="2" max="2" width="129.5546875" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1002,6 +1011,9 @@
       <c r="B2" t="s">
         <v>128</v>
       </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1010,6 +1022,9 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1018,6 +1033,9 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
+      <c r="C4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1026,6 +1044,9 @@
       <c r="B5" t="s">
         <v>127</v>
       </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1034,6 +1055,9 @@
       <c r="B6" t="s">
         <v>58</v>
       </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1042,6 +1066,9 @@
       <c r="B7" t="s">
         <v>57</v>
       </c>
+      <c r="C7" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1050,6 +1077,9 @@
       <c r="B8" t="s">
         <v>56</v>
       </c>
+      <c r="C8" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1057,6 +1087,9 @@
       </c>
       <c r="B9" t="s">
         <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>